<commit_message>
set locale for english us
</commit_message>
<xml_diff>
--- a/src/test/java/io/github/agache41/ormpipes/pipes/spreadSheet/cellstyle/xslx/multisheet/ExcelManySheetTest.xlsx
+++ b/src/test/java/io/github/agache41/ormpipes/pipes/spreadSheet/cellstyle/xslx/multisheet/ExcelManySheetTest.xlsx
@@ -637,9 +637,9 @@
   <sheetFormatPr defaultRowHeight="30.0" baseColWidth="30" customHeight="true"/>
   <cols>
     <col min="5" max="5" width="8.54296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.38671875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.98046875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.40625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.98828125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.14453125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.71875" customWidth="true"/>
     <col min="10" max="10" width="23.4375" customWidth="true"/>
   </cols>
@@ -753,9 +753,9 @@
   <cols>
     <col min="4" max="4" width="7.21484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="8.54296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.38671875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.98046875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.40625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.98828125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.14453125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.32421875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="12.32421875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="15.8203125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
fixed unit test, upgrade apache poi
</commit_message>
<xml_diff>
--- a/src/test/java/io/github/agache41/ormpipes/pipes/spreadSheet/cellstyle/xslx/multisheet/ExcelManySheetTest.xlsx
+++ b/src/test/java/io/github/agache41/ormpipes/pipes/spreadSheet/cellstyle/xslx/multisheet/ExcelManySheetTest.xlsx
@@ -636,10 +636,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.0" baseColWidth="30" customHeight="true"/>
   <cols>
-    <col min="5" max="5" width="8.54296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.40625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.98828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.14453125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="7.66015625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="12.0234375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.05859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="9.99609375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.71875" customWidth="true"/>
     <col min="10" max="10" width="23.4375" customWidth="true"/>
   </cols>
@@ -751,14 +751,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40.0" baseColWidth="40" customHeight="true"/>
   <cols>
-    <col min="4" max="4" width="7.21484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.54296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.40625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.98828125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.14453125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.32421875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="12.32421875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="15.8203125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.46875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="7.66015625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="12.0234375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.05859375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="9.99609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="14.1875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="40.0" customHeight="true"/>

</xml_diff>